<commit_message>
palabras filtro: rede de monitoeo y calidad del agua
</commit_message>
<xml_diff>
--- a/10 Curso de maestría.xlsx
+++ b/10 Curso de maestría.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Curso de maestría</t>
   </si>
@@ -25,7 +25,13 @@
     <t>Posgrado en Aprovechamiento de Recursos Hidráulicos</t>
   </si>
   <si>
+    <t>Grupo de Investigación en Recursos Hídricos y Saneamiento Ambiental</t>
+  </si>
+  <si>
     <t>40.- Nombre del Curso: Control y monitoreo de la calidad de cuerpos de agua Fecha acto administrativo curso: 2008-09-01 Número acto administrativo curso: 13 Programa académico: Maestria en Ingeniería - Recursos Hidraulicos</t>
+  </si>
+  <si>
+    <t>5.- Nombre del Curso: Monitoreo y Evaluación de la Calidad del Agua Fecha acto administrativo curso: 2017-12-05 Número acto administrativo curso: 318 Programa académico: Maestría en Ingeniería Civil</t>
   </si>
 </sst>
 </file>
@@ -383,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,7 +408,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>